<commit_message>
non_uniform_setup and exchange scripts and outputs
</commit_message>
<xml_diff>
--- a/imp_exp_hydro/Synthetic_Path_data.xlsx
+++ b/imp_exp_hydro/Synthetic_Path_data.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/sdenaro_ad_unc_edu/Documents/UNC_2017/Dispatch_model/PNW_Dispatch/imp_exp_hydro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdenaro\OneDrive - University of North Carolina at Chapel Hill\UNC_2017\Dispatch_model\PNW_Dispatch\imp_exp_hydro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7030"/>
   </bookViews>
   <sheets>
-    <sheet name="Synthetic_Path_data" sheetId="1" r:id="rId1"/>
+    <sheet name="2010" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -843,7 +843,7 @@
   <dimension ref="A1:E366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>